<commit_message>
add pom  and script classes for login and register user
</commit_message>
<xml_diff>
--- a/Resorses/234.xlsx
+++ b/Resorses/234.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkris\eclipse-vineela-workspace\AutomationExercise\Resorses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FCB700-7C72-44F3-AC42-2EDFF5E0D43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DA369A-212E-49FE-8903-2BFABC590E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4452" yWindow="2520" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,16 +33,16 @@
     <t>email</t>
   </si>
   <si>
-    <t>vineela123</t>
-  </si>
-  <si>
-    <t>vineela123@gmail.com</t>
-  </si>
-  <si>
-    <t>rajasri123</t>
-  </si>
-  <si>
-    <t>rajasr123i@gmail.com</t>
+    <t>rajasri1213</t>
+  </si>
+  <si>
+    <t>rajasr13423i@gmail.com</t>
+  </si>
+  <si>
+    <t>vineela12563</t>
+  </si>
+  <si>
+    <t>vineela125673@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -374,7 +374,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -389,18 +389,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>